<commit_message>
calibratie met een k
</commit_message>
<xml_diff>
--- a/src/NTC/Calibratie.xlsx
+++ b/src/NTC/Calibratie.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tymek\Documents\School\HardwareInterfacing\caseStudy\his\src\NTC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04BD14BC-40C2-4AD0-980D-62D4DCE3C4A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF8BB28-E21E-46D2-A784-9330607B8B00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2865" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -418,8 +418,13 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="nl-NL"/>
-                  <a:t>weerdstand</a:t>
+                  <a:t>weerdstand in</a:t>
                 </a:r>
+                <a:r>
+                  <a:rPr lang="nl-NL" baseline="0"/>
+                  <a:t> ohm</a:t>
+                </a:r>
+                <a:endParaRPr lang="nl-NL"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -725,7 +730,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -734,7 +739,7 @@
     <col min="4" max="4" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" t="s">
         <v>0</v>
@@ -751,7 +756,7 @@
         <v>2.3780000000000001E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
@@ -765,7 +770,7 @@
         <v>2.019E-7</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>-24</v>
       </c>
@@ -781,7 +786,7 @@
         <v>-23.295474580803216</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>-14</v>
       </c>
@@ -797,7 +802,7 @@
         <v>-14.778590706633452</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>-5</v>
       </c>
@@ -813,7 +818,7 @@
         <v>-4.730092096550095</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>0</v>
       </c>
@@ -829,7 +834,7 @@
         <v>0.32635677910212735</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>21</v>
       </c>
@@ -845,7 +850,7 @@
         <v>21.404803436929456</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>25</v>
       </c>
@@ -861,7 +866,7 @@
         <v>25.388752905373053</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>30</v>
       </c>
@@ -877,7 +882,7 @@
         <v>31.73759017684489</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>35</v>
       </c>

</xml_diff>